<commit_message>
Climbing stairs 2 solutions
</commit_message>
<xml_diff>
--- a/amazon-problems.xlsx
+++ b/amazon-problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://upm365-my.sharepoint.com/personal/g_vargash_alumnos_upm_es/Documents/Documentos/Github/Amazon Coding Interviews/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="476" documentId="8_{62C2EA49-8340-49A3-B68E-FC74A596A25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E39215E7-61AC-4F8B-AF0E-71031BF4A98A}"/>
+  <xr:revisionPtr revIDLastSave="485" documentId="8_{62C2EA49-8340-49A3-B68E-FC74A596A25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AEED28E-18C0-44EC-B533-192C4116B8BF}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11325" xr2:uid="{20102F37-584B-44CD-9965-569F7B7A1F21}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{20102F37-584B-44CD-9965-569F7B7A1F21}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="178">
   <si>
     <t>N</t>
   </si>
@@ -565,6 +565,9 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>C / Python</t>
   </si>
 </sst>
 </file>
@@ -1056,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A45CC4A8-B22F-4F1C-A6CC-AD15CCB51EEE}">
   <dimension ref="B2:K84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,7 +1145,7 @@
       </c>
       <c r="K4" s="3">
         <f>SUM(H8,H15,H32,H44:H46,H51:H52,H80)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1215,7 +1218,7 @@
       </c>
       <c r="K7" s="25">
         <f>SUM(K4:K6)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
@@ -1884,18 +1887,22 @@
       <c r="B46" s="7">
         <v>44</v>
       </c>
-      <c r="C46" s="24" t="s">
+      <c r="C46" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D46" s="18">
         <v>13</v>
       </c>
-      <c r="E46" s="9" t="s">
+      <c r="E46" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="F46" s="15"/>
+      <c r="F46" s="20" t="s">
+        <v>170</v>
+      </c>
       <c r="G46" s="12"/>
-      <c r="H46" s="23"/>
+      <c r="H46" s="22">
+        <v>1</v>
+      </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="7">
@@ -1969,18 +1976,22 @@
       <c r="B51" s="7">
         <v>49</v>
       </c>
-      <c r="C51" s="24" t="s">
+      <c r="C51" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="D51" s="3">
+      <c r="D51" s="18">
         <v>11</v>
       </c>
-      <c r="E51" s="9" t="s">
+      <c r="E51" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="F51" s="15"/>
+      <c r="F51" s="20" t="s">
+        <v>177</v>
+      </c>
       <c r="G51" s="12"/>
-      <c r="H51" s="23"/>
+      <c r="H51" s="22">
+        <v>1</v>
+      </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" s="7">
@@ -2616,8 +2627,5 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId82"/>
-  <ignoredErrors>
-    <ignoredError sqref="K4" formulaRange="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>